<commit_message>
planilha de quantidade de alunos formatada
</commit_message>
<xml_diff>
--- a/QuantidadeAlunos.xlsx
+++ b/QuantidadeAlunos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criscia.menezes\Desktop\Análises - Consumos de água e energia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\NOM\obras\Cris\Repo\BIProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5001E28A-E3DF-4C32-8B17-38E8E1893E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D9F19C-150A-4A86-9204-19956ADFE228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Quantidade de Alunos" sheetId="1" r:id="rId1"/>
+    <sheet name="QuantidadeAlunos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -333,13 +333,13 @@
     <t>WASHIGTON LUIZ DR.</t>
   </si>
   <si>
-    <t>QuantidadeAlunos</t>
-  </si>
-  <si>
-    <t>CodigoCIE</t>
-  </si>
-  <si>
-    <t>UnidadeEscolar</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>SchoolUnit</t>
+  </si>
+  <si>
+    <t>NumberOfStudents</t>
   </si>
 </sst>
 </file>
@@ -693,7 +693,7 @@
   <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,13 +705,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>